<commit_message>
meta yaml schema done simplified for now
</commit_message>
<xml_diff>
--- a/metadata/animals_template.xlsx
+++ b/metadata/animals_template.xlsx
@@ -7,11 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="animals" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="sessions" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="functional_stack" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="anatomy_stack" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="channels" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="stacks" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -21,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -38,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -46,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -417,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:X1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,283 +434,124 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>animal_id</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>genotype</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>owner</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>tank</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>date_of_birth</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>meta_source_type</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>meta_source_path</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>root_dir</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>functional_2p</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>anatomy_2p</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>confocal_rounds</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>behavior</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>animal_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>session_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>session_type</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>stack_id</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>stack_type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>date</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>condition</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>experimenter</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>include_in_analysis</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>image_quality</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>notes</t>
         </is>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>session_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>raw_path</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>microscope_settings_path</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>stimulus_name</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>stimulus_metadata_path</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>microscope_settings_path</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>num_planes</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>zoom_factor</t>
         </is>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>session_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>round_id</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>raw_path</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>plane_spacing</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>microscope_settings_path</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>session_id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>round_id</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>channel_id</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>marker</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>wavelength_nm</t>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>reference_channel_index</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>channel1_name</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>channel1_wavelength_nm</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>channel2_name</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>channel2_wavelength_nm</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>channel3_name</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>channel3_wavelength_nm</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update metadata with 2p parameters for preprocessing
</commit_message>
<xml_diff>
--- a/metadata/animals_template.xlsx
+++ b/metadata/animals_template.xlsx
@@ -7,7 +7,9 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="stacks" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="animals" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="stacks" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="two_photon_settings" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,6 +443,57 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>genotype</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>owner</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>tank</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>date_of_birth</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>root_dir</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:V1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>animal_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>stack_id</t>
         </is>
       </c>
@@ -486,72 +539,118 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>microscope_settings_path</t>
+          <t>stimulus_name</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>stimulus_name</t>
+          <t>stimulus_metadata_path</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>stimulus_metadata_path</t>
+          <t>zoom_factor</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>num_planes</t>
+          <t>round_id</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>zoom_factor</t>
+          <t>plane_spacing</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>round_id</t>
+          <t>reference_channel_index</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>plane_spacing</t>
+          <t>channel1_name</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>reference_channel_index</t>
+          <t>channel1_wavelength_nm</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>channel1_name</t>
+          <t>channel2_name</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>channel1_wavelength_nm</t>
+          <t>channel2_wavelength_nm</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>channel2_name</t>
+          <t>channel3_name</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>channel2_wavelength_nm</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>channel3_name</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
           <t>channel3_wavelength_nm</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>session_id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>mode</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>n_planes</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>frames_per_plane</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>flyback_frames</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>remove_first_frame</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>blocks</t>
         </is>
       </c>
     </row>

</xml_diff>